<commit_message>
updating iNEXT code after package updates
</commit_message>
<xml_diff>
--- a/figures_tables/Table_S4.xlsx
+++ b/figures_tables/Table_S4.xlsx
@@ -123,22 +123,22 @@
         <v>7</v>
       </c>
       <c r="B2" t="n">
-        <v>1.991666666666666</v>
+        <v>2.1716685820065127</v>
       </c>
       <c r="C2" t="n">
-        <v>1.9410242427932505</v>
+        <v>2.00124302412812</v>
       </c>
       <c r="D2" t="n">
-        <v>4.628666666666667</v>
+        <v>4.718067388696906</v>
       </c>
       <c r="E2" t="n">
-        <v>1.388063559223584</v>
+        <v>1.351231779597265</v>
       </c>
       <c r="F2" t="n">
-        <v>5.334333333333334</v>
+        <v>5.398287328394347</v>
       </c>
       <c r="G2" t="n">
-        <v>1.3185234586882064</v>
+        <v>1.2872725023091371</v>
       </c>
     </row>
     <row r="3">
@@ -146,22 +146,22 @@
         <v>8</v>
       </c>
       <c r="B3" t="n">
-        <v>1.6535000000000002</v>
+        <v>1.5284257587900505</v>
       </c>
       <c r="C3" t="n">
-        <v>1.003917949834547</v>
+        <v>0.9849155338944934</v>
       </c>
       <c r="D3" t="n">
-        <v>3.679833333333333</v>
+        <v>3.5999748924387234</v>
       </c>
       <c r="E3" t="n">
-        <v>0.9446390286476865</v>
+        <v>0.9203589835436573</v>
       </c>
       <c r="F3" t="n">
-        <v>4.2971666666666675</v>
+        <v>4.247972640506182</v>
       </c>
       <c r="G3" t="n">
-        <v>0.9973578901834143</v>
+        <v>0.9774366686076593</v>
       </c>
     </row>
     <row r="4">
@@ -169,22 +169,22 @@
         <v>9</v>
       </c>
       <c r="B4" t="n">
-        <v>5.8622499999999995</v>
+        <v>5.878683605029869</v>
       </c>
       <c r="C4" t="n">
-        <v>0.811666226043686</v>
+        <v>0.8023107209044661</v>
       </c>
       <c r="D4" t="n">
-        <v>4.99775</v>
+        <v>5.008172886841643</v>
       </c>
       <c r="E4" t="n">
-        <v>0.4508514860793962</v>
+        <v>0.4578169882560387</v>
       </c>
       <c r="F4" t="n">
-        <v>4.39025</v>
+        <v>4.396447212636887</v>
       </c>
       <c r="G4" t="n">
-        <v>0.7816352916588827</v>
+        <v>0.7869921693224223</v>
       </c>
     </row>
     <row r="5">
@@ -192,22 +192,22 @@
         <v>10</v>
       </c>
       <c r="B5" t="n">
-        <v>4.468999999999999</v>
+        <v>4.65059330644514</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7238534612290897</v>
+        <v>0.7913677463237762</v>
       </c>
       <c r="D5" t="n">
-        <v>4.2995</v>
+        <v>4.370886260119848</v>
       </c>
       <c r="E5" t="n">
-        <v>1.025428081339691</v>
+        <v>1.061707234163964</v>
       </c>
       <c r="F5" t="n">
-        <v>4.09725</v>
+        <v>4.136227690441243</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9799411015464142</v>
+        <v>1.0002426955902959</v>
       </c>
     </row>
   </sheetData>

</xml_diff>